<commit_message>
Very small spreadsheet update :P
</commit_message>
<xml_diff>
--- a/other/Crafting recipe brainstorm.xlsx
+++ b/other/Crafting recipe brainstorm.xlsx
@@ -29,15 +29,6 @@
     <t>Enderperlite &gt; EnperToolMaterial</t>
   </si>
   <si>
-    <t>Step 1</t>
-  </si>
-  <si>
-    <t>Step 2</t>
-  </si>
-  <si>
-    <t>Step 3</t>
-  </si>
-  <si>
     <t>e = endper</t>
   </si>
   <si>
@@ -99,6 +90,15 @@
   </si>
   <si>
     <t>e3= endpertoolmaterial</t>
+  </si>
+  <si>
+    <t>Step 1 Heating</t>
+  </si>
+  <si>
+    <t>Step 2 Cutting</t>
+  </si>
+  <si>
+    <t>Step 3 Cooling</t>
   </si>
 </sst>
 </file>
@@ -143,14 +143,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="H9:V23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,158 +453,158 @@
   </cols>
   <sheetData>
     <row r="9" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
     </row>
     <row r="10" spans="12:22" x14ac:dyDescent="0.25">
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="1"/>
-      <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
     </row>
     <row r="12" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L12" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="P12" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="T12" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="12:22" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L13" s="2" t="s">
+      <c r="L13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="P13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>8</v>
+      </c>
+      <c r="R13" t="s">
+        <v>7</v>
+      </c>
+      <c r="T13" t="s">
         <v>15</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="P13" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>11</v>
-      </c>
-      <c r="R13" t="s">
-        <v>10</v>
-      </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
+        <v>14</v>
+      </c>
+      <c r="V13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="12:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="P14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" t="s">
+        <v>6</v>
+      </c>
+      <c r="T14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" t="s">
+        <v>13</v>
+      </c>
+      <c r="V14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="12:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="P15" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" t="s">
+        <v>5</v>
+      </c>
+      <c r="T15" t="s">
+        <v>15</v>
+      </c>
+      <c r="U15" t="s">
+        <v>14</v>
+      </c>
+      <c r="V15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="8:21" x14ac:dyDescent="0.25">
+      <c r="M17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U13" t="s">
-        <v>17</v>
-      </c>
-      <c r="V13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="12:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="P14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>7</v>
-      </c>
-      <c r="R14" t="s">
-        <v>9</v>
-      </c>
-      <c r="T14" t="s">
-        <v>16</v>
-      </c>
-      <c r="U14" t="s">
-        <v>16</v>
-      </c>
-      <c r="V14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="12:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="P15" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>12</v>
-      </c>
-      <c r="R15" t="s">
-        <v>8</v>
-      </c>
-      <c r="T15" t="s">
-        <v>18</v>
-      </c>
-      <c r="U15" t="s">
-        <v>17</v>
-      </c>
-      <c r="V15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="8:21" x14ac:dyDescent="0.25">
-      <c r="M17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="U17" s="4" t="s">
-        <v>23</v>
+      <c r="Q17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="8:21" x14ac:dyDescent="0.25">
       <c r="L19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="T19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H20" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="T20" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="8:21" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>